<commit_message>
remove log4j jar - vulnerability found in pom.xml
</commit_message>
<xml_diff>
--- a/src/main/java/com/testdata/SambaSafety_testdata.xlsx
+++ b/src/main/java/com/testdata/SambaSafety_testdata.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="94">
   <si>
     <t>FirstName</t>
   </si>
@@ -297,6 +297,18 @@
   </si>
   <si>
     <t>21-09-2020 10:56:47</t>
+  </si>
+  <si>
+    <t>21-09-2020 11:38:0</t>
+  </si>
+  <si>
+    <t>21-09-2020 11:38:3</t>
+  </si>
+  <si>
+    <t>21-09-2020 11:38:7</t>
+  </si>
+  <si>
+    <t>21-09-2020 11:38:10</t>
   </si>
 </sst>
 </file>
@@ -717,7 +729,7 @@
   <cols>
     <col min="1" max="1" customWidth="true" style="3" width="39.7265625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="6.59375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="27.66015625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="19.66796875" collapsed="true"/>
     <col min="4" max="16384" style="3" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
@@ -740,7 +752,7 @@
         <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -751,7 +763,7 @@
         <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -762,7 +774,7 @@
         <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -773,7 +785,7 @@
         <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add log4j and update testng.xml
</commit_message>
<xml_diff>
--- a/src/main/java/com/testdata/SambaSafety_testdata.xlsx
+++ b/src/main/java/com/testdata/SambaSafety_testdata.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="98">
   <si>
     <t>FirstName</t>
   </si>
@@ -309,6 +309,18 @@
   </si>
   <si>
     <t>21-09-2020 11:38:10</t>
+  </si>
+  <si>
+    <t>22-09-2020 01:52:22</t>
+  </si>
+  <si>
+    <t>22-09-2020 01:52:28</t>
+  </si>
+  <si>
+    <t>22-09-2020 01:52:32</t>
+  </si>
+  <si>
+    <t>22-09-2020 01:52:38</t>
   </si>
 </sst>
 </file>
@@ -752,7 +764,7 @@
         <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -763,7 +775,7 @@
         <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -774,7 +786,7 @@
         <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -785,7 +797,7 @@
         <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>